<commit_message>
FIX THÀNH CÔNG WEB DÙNG GUID
</commit_message>
<xml_diff>
--- a/MauImport/MauImportQLTS - Copy.xlsx
+++ b/MauImport/MauImportQLTS - Copy.xlsx
@@ -7,30 +7,30 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="ViTri" sheetId="3" r:id="rId1"/>
-    <sheet name="NhanVienPT" sheetId="4" r:id="rId2"/>
-    <sheet name="Phong" sheetId="8" r:id="rId3"/>
-    <sheet name="LoaiThietBi" sheetId="5" r:id="rId4"/>
-    <sheet name="TinhTrang" sheetId="9" r:id="rId5"/>
-    <sheet name="ThietBiChung" sheetId="6" r:id="rId6"/>
-    <sheet name="ThietBiRieng" sheetId="10" r:id="rId7"/>
+    <sheet sheetId="3" r:id="rId1" name="ViTri"/>
+    <sheet sheetId="4" r:id="rId2" name="NhanVienPT"/>
+    <sheet sheetId="8" r:id="rId3" name="Phong"/>
+    <sheet sheetId="5" r:id="rId4" name="LoaiThietBi"/>
+    <sheet sheetId="9" r:id="rId5" name="TinhTrang"/>
+    <sheet sheetId="6" r:id="rId6" name="ThietBiChung"/>
+    <sheet sheetId="10" r:id="rId7" name="ThietBiRieng"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ViTri!$C$2:$C$18</definedName>
     <definedName name="Coso">#REF!:INDEX(#REF!,#REF!)</definedName>
     <definedName name="Day">#REF!:INDEX(#REF!,#REF!)</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="0">ViTri!$D$3</definedName>
     <definedName name="ListCoSo">#REF!</definedName>
     <definedName name="ListDay">#REF!</definedName>
     <definedName name="ListTang">#REF!</definedName>
-    <definedName name="MaNhanVien">NhanVienPT!$B$2:$B$2995</definedName>
-    <definedName name="NhanVien">NhanVienPT!$C$2:$C$2995</definedName>
     <definedName name="Tang">#REF!:INDEX(#REF!,#REF!)</definedName>
     <definedName name="UniqueCoSo">ViTri!$C$2:INDEX(ViTri!$C$2:$C$2001,COUNTA(ViTri!$C$2:$C$2001))</definedName>
     <definedName name="UniqueDay">ViTri!$E$2:INDEX(ViTri!$E$2:$E$2001,COUNTA(ViTri!$E$2:$E$2001))</definedName>
     <definedName name="UniqueTang">ViTri!$G$2:INDEX(ViTri!$G$2:$G$2001,COUNTA(ViTri!$G$2:$G$2001))</definedName>
+    <definedName name="_xlnm._FilterDatabase">ViTri!$C$2:$C$18</definedName>
+    <definedName name="_xlnm.Extract">ViTri!$D$3</definedName>
+    <definedName name="MaNhanVien">NhanVienPT!$B$2:$B$2995</definedName>
+    <definedName name="NhanVien">NhanVienPT!$C$2:$C$2995</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" fullCalcOnLoad="true"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1021,15 +1021,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0" rightToLeft="false">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1047,7 +1047,7 @@
     <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row spans="1:28" s="14" customFormat="1" outlineLevel="0" r="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row spans="1:28" outlineLevel="0" r="2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1109,9 +1109,13 @@
       <c r="J2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="24"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K2" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1134,9 +1138,13 @@
       <c r="J3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K3" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="4">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1164,9 +1172,13 @@
       <c r="J4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K4" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="5">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1194,9 +1206,13 @@
       <c r="J5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="24"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K5" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="6">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1224,9 +1240,13 @@
       <c r="J6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="24"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K6" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="7">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1249,9 +1269,13 @@
       <c r="J7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K7" s="24"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K7" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="8">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -1279,9 +1303,13 @@
       <c r="J8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="24"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K8" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="9">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1309,9 +1337,13 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="24"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K9" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="10">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1339,9 +1371,13 @@
       <c r="J10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="24"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K10" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="11">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1369,9 +1405,13 @@
       <c r="J11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="24"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K11" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="12">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1394,9 +1434,13 @@
       <c r="J12" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K12" s="24"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K12" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="13">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1424,19 +1468,23 @@
       <c r="J13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="K13" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="14">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row spans="1:28" outlineLevel="0" r="15">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row spans="1:28" outlineLevel="0" r="16">
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Thay đổi thông tin host lưu file docx
Thay đổi thông tin host lưu file docx
Thêm file import cấu hình
edit 1 vài thứ linh tinh
</commit_message>
<xml_diff>
--- a/MauImport/MauImportQLTS - Copy.xlsx
+++ b/MauImport/MauImportQLTS - Copy.xlsx
@@ -1,37 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="3" r:id="rId1" name="ViTri"/>
-    <sheet sheetId="4" r:id="rId2" name="NhanVienPT"/>
-    <sheet sheetId="8" r:id="rId3" name="Phong"/>
-    <sheet sheetId="5" r:id="rId4" name="LoaiThietBi"/>
-    <sheet sheetId="9" r:id="rId5" name="TinhTrang"/>
-    <sheet sheetId="6" r:id="rId6" name="ThietBiChung"/>
-    <sheet sheetId="10" r:id="rId7" name="ThietBiRieng"/>
+    <sheet name="ViTri" sheetId="3" r:id="rId1"/>
+    <sheet name="NhanVienPT" sheetId="4" r:id="rId2"/>
+    <sheet name="Phong" sheetId="8" r:id="rId3"/>
+    <sheet name="LoaiThietBi" sheetId="5" r:id="rId4"/>
+    <sheet name="TinhTrang" sheetId="9" r:id="rId5"/>
+    <sheet name="ThietBiChung" sheetId="6" r:id="rId6"/>
+    <sheet name="ThietBiRieng" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase">ViTri!$C$2:$C$18</definedName>
     <definedName name="Coso">#REF!:INDEX(#REF!,#REF!)</definedName>
     <definedName name="Day">#REF!:INDEX(#REF!,#REF!)</definedName>
+    <definedName name="_xlnm.Extract">ViTri!$D$3</definedName>
     <definedName name="ListCoSo">#REF!</definedName>
     <definedName name="ListDay">#REF!</definedName>
     <definedName name="ListTang">#REF!</definedName>
+    <definedName name="MaNhanVien">NhanVienPT!$B$2:$B$2995</definedName>
+    <definedName name="NhanVien">NhanVienPT!$C$2:$C$2995</definedName>
     <definedName name="Tang">#REF!:INDEX(#REF!,#REF!)</definedName>
     <definedName name="UniqueCoSo">ViTri!$C$2:INDEX(ViTri!$C$2:$C$2001,COUNTA(ViTri!$C$2:$C$2001))</definedName>
     <definedName name="UniqueDay">ViTri!$E$2:INDEX(ViTri!$E$2:$E$2001,COUNTA(ViTri!$E$2:$E$2001))</definedName>
     <definedName name="UniqueTang">ViTri!$G$2:INDEX(ViTri!$G$2:$G$2001,COUNTA(ViTri!$G$2:$G$2001))</definedName>
-    <definedName name="_xlnm._FilterDatabase">ViTri!$C$2:$C$18</definedName>
-    <definedName name="_xlnm.Extract">ViTri!$D$3</definedName>
-    <definedName name="MaNhanVien">NhanVienPT!$B$2:$B$2995</definedName>
-    <definedName name="NhanVien">NhanVienPT!$C$2:$C$2995</definedName>
   </definedNames>
-  <calcPr calcId="144525" fullCalcOnLoad="true"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -601,11 +600,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,19 +1013,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0" rightToLeft="false">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1047,7 +1046,7 @@
     <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row spans="1:28" s="14" customFormat="1" outlineLevel="0" r="1">
+    <row r="1" spans="1:28" s="14" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row spans="1:28" outlineLevel="0" r="2">
+    <row r="2" spans="1:28">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1109,13 +1108,9 @@
       <c r="J2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="3">
+      <c r="K2" s="24"/>
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1138,13 +1133,9 @@
       <c r="J3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="4">
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:28">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1172,13 +1163,9 @@
       <c r="J4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K4" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="5">
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:28">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1206,13 +1193,9 @@
       <c r="J5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="6">
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:28">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1240,13 +1223,9 @@
       <c r="J6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="7">
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:28">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1269,13 +1248,9 @@
       <c r="J7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K7" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="8">
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:28">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -1303,13 +1278,9 @@
       <c r="J8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="9">
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:28">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1337,13 +1308,9 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="10">
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:28">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1371,13 +1338,9 @@
       <c r="J10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="11">
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:28">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1405,13 +1368,9 @@
       <c r="J11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="12">
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:28">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1434,13 +1393,9 @@
       <c r="J12" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K12" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="13">
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:28">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1468,23 +1423,19 @@
       <c r="J13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K13" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:28" outlineLevel="0" r="14">
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:28">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row spans="1:28" outlineLevel="0" r="15">
+    <row r="15" spans="1:28">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row spans="1:28" outlineLevel="0" r="16">
+    <row r="16" spans="1:28">
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
@@ -1500,7 +1451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1508,7 +1459,7 @@
       <selection pane="bottomLeft" activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1519,7 +1470,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="14" customFormat="1">
       <c r="A1" s="15" t="s">
         <v>182</v>
       </c>
@@ -1542,7 +1493,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1557,7 +1508,7 @@
       </c>
       <c r="G2" s="24"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1572,7 +1523,7 @@
       </c>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1587,7 +1538,7 @@
       </c>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1602,7 +1553,7 @@
       </c>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1623,15 +1574,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1647,7 +1598,7 @@
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="14" customFormat="1">
       <c r="A1" s="15" t="s">
         <v>182</v>
       </c>
@@ -1685,7 +1636,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1709,7 +1660,7 @@
       </c>
       <c r="L2" s="24"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -1733,7 +1684,7 @@
       </c>
       <c r="L3" s="24"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -1757,7 +1708,7 @@
       </c>
       <c r="L4" s="24"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -1782,7 +1733,7 @@
       </c>
       <c r="L5" s="24"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -1807,7 +1758,7 @@
       </c>
       <c r="L6" s="24"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -1832,7 +1783,7 @@
       </c>
       <c r="L7" s="24"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -1853,7 +1804,7 @@
       </c>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -1874,7 +1825,7 @@
       </c>
       <c r="L9" s="24"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -1895,7 +1846,7 @@
       </c>
       <c r="L10" s="24"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -1920,7 +1871,7 @@
       </c>
       <c r="L11" s="24"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -1945,7 +1896,7 @@
       </c>
       <c r="L12" s="24"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -1970,7 +1921,7 @@
       </c>
       <c r="L13" s="24"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -1995,7 +1946,7 @@
       </c>
       <c r="L14" s="24"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -2020,7 +1971,7 @@
       </c>
       <c r="L15" s="24"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -2045,7 +1996,7 @@
       </c>
       <c r="L16" s="24"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -2070,7 +2021,7 @@
       </c>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -2095,7 +2046,7 @@
       </c>
       <c r="L18" s="24"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -2120,7 +2071,7 @@
       </c>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -2145,7 +2096,7 @@
       </c>
       <c r="L20" s="24"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="23">
         <v>20</v>
       </c>
@@ -2170,7 +2121,7 @@
       </c>
       <c r="L21" s="24"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="23">
         <v>21</v>
       </c>
@@ -2195,7 +2146,7 @@
       </c>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="23">
         <v>22</v>
       </c>
@@ -2220,7 +2171,7 @@
       </c>
       <c r="L23" s="24"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="23">
         <v>23</v>
       </c>
@@ -2245,7 +2196,7 @@
       </c>
       <c r="L24" s="24"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="23">
         <v>24</v>
       </c>
@@ -2270,7 +2221,7 @@
       </c>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="23">
         <v>25</v>
       </c>
@@ -2295,7 +2246,7 @@
       </c>
       <c r="L26" s="24"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="23">
         <v>26</v>
       </c>
@@ -2320,7 +2271,7 @@
       </c>
       <c r="L27" s="24"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="23">
         <v>27</v>
       </c>
@@ -2345,7 +2296,7 @@
       </c>
       <c r="L28" s="24"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="23">
         <v>28</v>
       </c>
@@ -2370,7 +2321,7 @@
       </c>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="23">
         <v>29</v>
       </c>
@@ -2395,7 +2346,7 @@
       </c>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="23">
         <v>30</v>
       </c>
@@ -2420,7 +2371,7 @@
       </c>
       <c r="L31" s="24"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="23">
         <v>31</v>
       </c>
@@ -2445,7 +2396,7 @@
       </c>
       <c r="L32" s="24"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="23">
         <v>32</v>
       </c>
@@ -2470,7 +2421,7 @@
       </c>
       <c r="L33" s="24"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="23">
         <v>33</v>
       </c>
@@ -2495,7 +2446,7 @@
       </c>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="23">
         <v>34</v>
       </c>
@@ -2520,7 +2471,7 @@
       </c>
       <c r="L35" s="24"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="23">
         <v>35</v>
       </c>
@@ -2542,7 +2493,7 @@
       </c>
       <c r="L36" s="24"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="23">
         <v>36</v>
       </c>
@@ -2564,7 +2515,7 @@
       </c>
       <c r="L37" s="24"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="23">
         <v>37</v>
       </c>
@@ -2586,7 +2537,7 @@
       </c>
       <c r="L38" s="24"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="23">
         <v>38</v>
       </c>
@@ -2608,7 +2559,7 @@
       </c>
       <c r="L39" s="24"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="23">
         <v>39</v>
       </c>
@@ -2630,7 +2581,7 @@
       </c>
       <c r="L40" s="24"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="23">
         <v>40</v>
       </c>
@@ -2648,14 +2599,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="2" bestFit="1" customWidth="1"/>
@@ -2666,7 +2617,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="13" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -2689,7 +2640,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2701,7 +2652,7 @@
       </c>
       <c r="G2" s="24"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2713,7 +2664,7 @@
       </c>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2725,7 +2676,7 @@
       </c>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2737,7 +2688,7 @@
       </c>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2755,14 +2706,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="2" customWidth="1"/>
@@ -2774,7 +2725,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="13" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -2790,7 +2741,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2803,7 +2754,7 @@
       </c>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2816,7 +2767,7 @@
       </c>
       <c r="D3" s="24"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2829,7 +2780,7 @@
       </c>
       <c r="D4" s="24"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2842,7 +2793,7 @@
       </c>
       <c r="D5" s="24"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2855,7 +2806,7 @@
       </c>
       <c r="D6" s="24"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2868,7 +2819,7 @@
       </c>
       <c r="D7" s="24"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -2881,7 +2832,7 @@
       </c>
       <c r="D8" s="24"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -2900,16 +2851,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="2" customWidth="1"/>
@@ -2924,7 +2875,7 @@
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="13" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -2954,7 +2905,7 @@
       </c>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2975,7 +2926,7 @@
       </c>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -2993,7 +2944,7 @@
       </c>
       <c r="I3" s="24"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -3011,7 +2962,7 @@
       </c>
       <c r="I4" s="24"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -3029,7 +2980,7 @@
       </c>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -3047,7 +2998,7 @@
       </c>
       <c r="I6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -3065,7 +3016,7 @@
       </c>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -3086,7 +3037,7 @@
       </c>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -3104,7 +3055,7 @@
       </c>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -3122,7 +3073,7 @@
       </c>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -3140,7 +3091,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -3158,7 +3109,7 @@
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -3176,7 +3127,7 @@
       </c>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -3194,7 +3145,7 @@
       </c>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -3212,7 +3163,7 @@
       </c>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -3230,7 +3181,7 @@
       </c>
       <c r="I16" s="24"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -3248,7 +3199,7 @@
       </c>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -3266,7 +3217,7 @@
       </c>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -3284,7 +3235,7 @@
       </c>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -3302,7 +3253,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="23">
         <v>20</v>
       </c>
@@ -3320,7 +3271,7 @@
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="23">
         <v>21</v>
       </c>
@@ -3338,7 +3289,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="23">
         <v>22</v>
       </c>
@@ -3356,7 +3307,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="23">
         <v>23</v>
       </c>
@@ -3377,7 +3328,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="23">
         <v>24</v>
       </c>
@@ -3395,7 +3346,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="23">
         <v>25</v>
       </c>
@@ -3413,7 +3364,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="23">
         <v>26</v>
       </c>
@@ -3431,7 +3382,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="23">
         <v>27</v>
       </c>
@@ -3449,7 +3400,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="23">
         <v>28</v>
       </c>
@@ -3467,7 +3418,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="23">
         <v>29</v>
       </c>
@@ -3485,7 +3436,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="23">
         <v>30</v>
       </c>
@@ -3503,7 +3454,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="23">
         <v>31</v>
       </c>
@@ -3521,7 +3472,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="23">
         <v>32</v>
       </c>
@@ -3539,7 +3490,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="23">
         <v>33</v>
       </c>
@@ -3557,7 +3508,7 @@
       </c>
       <c r="I34" s="24"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="23">
         <v>34</v>
       </c>
@@ -3582,14 +3533,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H40" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -3607,7 +3558,7 @@
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="13" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -3646,7 +3597,7 @@
       </c>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -3667,7 +3618,7 @@
       </c>
       <c r="L2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -3688,7 +3639,7 @@
       </c>
       <c r="L3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -3709,7 +3660,7 @@
       </c>
       <c r="L4" s="24"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -3730,7 +3681,7 @@
       </c>
       <c r="L5" s="24"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -3751,7 +3702,7 @@
       </c>
       <c r="L6" s="24"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -3772,7 +3723,7 @@
       </c>
       <c r="L7" s="24"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -3793,7 +3744,7 @@
       </c>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -3814,7 +3765,7 @@
       </c>
       <c r="L9" s="24"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -3835,7 +3786,7 @@
       </c>
       <c r="L10" s="24"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -3856,7 +3807,7 @@
       </c>
       <c r="L11" s="24"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -3874,7 +3825,7 @@
       </c>
       <c r="L12" s="24"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -3895,7 +3846,7 @@
       </c>
       <c r="L13" s="24"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -3916,7 +3867,7 @@
       </c>
       <c r="L14" s="24"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -3937,7 +3888,7 @@
       </c>
       <c r="L15" s="24"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -3958,7 +3909,7 @@
       </c>
       <c r="L16" s="24"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -3979,7 +3930,7 @@
       </c>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="23">
         <v>17</v>
       </c>
@@ -4000,7 +3951,7 @@
       </c>
       <c r="L18" s="24"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -4021,7 +3972,7 @@
       </c>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -4042,7 +3993,7 @@
       </c>
       <c r="L20" s="24"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="23">
         <v>20</v>
       </c>
@@ -4063,7 +4014,7 @@
       </c>
       <c r="L21" s="24"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="23">
         <v>21</v>
       </c>
@@ -4084,7 +4035,7 @@
       </c>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="23">
         <v>22</v>
       </c>
@@ -4105,7 +4056,7 @@
       </c>
       <c r="L23" s="24"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="23">
         <v>23</v>
       </c>
@@ -4123,7 +4074,7 @@
       </c>
       <c r="L24" s="24"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="23">
         <v>24</v>
       </c>
@@ -4141,7 +4092,7 @@
       </c>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="23">
         <v>25</v>
       </c>
@@ -4162,7 +4113,7 @@
       </c>
       <c r="L26" s="24"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="23">
         <v>26</v>
       </c>
@@ -4180,7 +4131,7 @@
       </c>
       <c r="L27" s="24"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="23">
         <v>27</v>
       </c>
@@ -4198,7 +4149,7 @@
       </c>
       <c r="L28" s="24"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="23">
         <v>28</v>
       </c>
@@ -4216,7 +4167,7 @@
       </c>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="23">
         <v>29</v>
       </c>
@@ -4237,7 +4188,7 @@
       </c>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="23">
         <v>30</v>
       </c>
@@ -4255,7 +4206,7 @@
       </c>
       <c r="L31" s="24"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="23">
         <v>31</v>
       </c>
@@ -4276,7 +4227,7 @@
       </c>
       <c r="L32" s="24"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="23">
         <v>32</v>
       </c>
@@ -4297,7 +4248,7 @@
       </c>
       <c r="L33" s="24"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="23">
         <v>33</v>
       </c>
@@ -4315,7 +4266,7 @@
       </c>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="23">
         <v>34</v>
       </c>
@@ -4336,7 +4287,7 @@
       </c>
       <c r="L35" s="24"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="23">
         <v>35</v>
       </c>
@@ -4357,7 +4308,7 @@
       </c>
       <c r="L36" s="24"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="23">
         <v>36</v>
       </c>
@@ -4378,7 +4329,7 @@
       </c>
       <c r="L37" s="24"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="23">
         <v>37</v>
       </c>
@@ -4399,7 +4350,7 @@
       </c>
       <c r="L38" s="24"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="23">
         <v>38</v>
       </c>
@@ -4420,7 +4371,7 @@
       </c>
       <c r="L39" s="24"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="23">
         <v>39</v>
       </c>
@@ -4441,7 +4392,7 @@
       </c>
       <c r="L40" s="24"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="23">
         <v>40</v>
       </c>
@@ -4462,7 +4413,7 @@
       </c>
       <c r="L41" s="24"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="23">
         <v>41</v>
       </c>
@@ -4483,7 +4434,7 @@
       </c>
       <c r="L42" s="24"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="23">
         <v>42</v>
       </c>
@@ -4504,7 +4455,7 @@
       </c>
       <c r="L43" s="24"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="23">
         <v>43</v>
       </c>
@@ -4525,7 +4476,7 @@
       </c>
       <c r="L44" s="24"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="23">
         <v>44</v>
       </c>
@@ -4546,7 +4497,7 @@
       </c>
       <c r="L45" s="24"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" s="23">
         <v>45</v>
       </c>
@@ -4567,7 +4518,7 @@
       </c>
       <c r="L46" s="24"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" s="23">
         <v>46</v>
       </c>
@@ -4588,7 +4539,7 @@
       </c>
       <c r="L47" s="24"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="23">
         <v>47</v>
       </c>
@@ -4609,7 +4560,7 @@
       </c>
       <c r="L48" s="24"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="23">
         <v>48</v>
       </c>
@@ -4630,7 +4581,7 @@
       </c>
       <c r="L49" s="24"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="23">
         <v>49</v>
       </c>
@@ -4651,7 +4602,7 @@
       </c>
       <c r="L50" s="24"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" s="23">
         <v>50</v>
       </c>
@@ -4672,7 +4623,7 @@
       </c>
       <c r="L51" s="24"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" s="23">
         <v>51</v>
       </c>
@@ -4693,7 +4644,7 @@
       </c>
       <c r="L52" s="24"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="23">
         <v>52</v>
       </c>
@@ -4714,7 +4665,7 @@
       </c>
       <c r="L53" s="24"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="23">
         <v>53</v>
       </c>
@@ -4735,7 +4686,7 @@
       </c>
       <c r="L54" s="24"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="23">
         <v>54</v>
       </c>
@@ -4756,7 +4707,7 @@
       </c>
       <c r="L55" s="24"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" s="23">
         <v>55</v>
       </c>
@@ -4777,7 +4728,7 @@
       </c>
       <c r="L56" s="24"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" s="23">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Đang fix toàn bộ Web dùng ucTreeList và fix lại cách hiển thị thông tin (không dùng textbox nữa)
</commit_message>
<xml_diff>
--- a/MauImport/MauImportQLTS - Copy.xlsx
+++ b/MauImport/MauImportQLTS - Copy.xlsx
@@ -1023,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0" rightToLeft="false">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2:K13"/>
     </sheetView>
@@ -1046,7 +1046,7 @@
     <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="14" customFormat="1">
+    <row spans="1:28" s="14" customFormat="1" outlineLevel="0" r="1">
       <c r="A1" s="10" t="s">
         <v>182</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row spans="1:28" outlineLevel="0" r="2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1108,9 +1108,13 @@
       <c r="J2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="24"/>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="K2" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1133,9 +1137,13 @@
       <c r="J3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:28">
+      <c r="K3" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="4">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1163,9 +1171,13 @@
       <c r="J4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="K4" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="5">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1193,9 +1205,13 @@
       <c r="J5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="24"/>
-    </row>
-    <row r="6" spans="1:28">
+      <c r="K5" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="6">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1223,9 +1239,13 @@
       <c r="J6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="24"/>
-    </row>
-    <row r="7" spans="1:28">
+      <c r="K6" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="7">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1248,9 +1268,13 @@
       <c r="J7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K7" s="24"/>
-    </row>
-    <row r="8" spans="1:28">
+      <c r="K7" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="8">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -1278,9 +1302,13 @@
       <c r="J8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="24"/>
-    </row>
-    <row r="9" spans="1:28">
+      <c r="K8" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="9">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1308,9 +1336,13 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="24"/>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="K9" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="10">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1338,9 +1370,13 @@
       <c r="J10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="24"/>
-    </row>
-    <row r="11" spans="1:28">
+      <c r="K10" s="24" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:28" outlineLevel="0" r="11">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1370,7 +1406,7 @@
       </c>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="1:28">
+    <row spans="1:28" outlineLevel="0" r="12">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1395,7 +1431,7 @@
       </c>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="1:28">
+    <row spans="1:28" outlineLevel="0" r="13">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1425,17 +1461,17 @@
       </c>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="1:28">
+    <row spans="1:28" outlineLevel="0" r="14">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:28">
+    <row spans="1:28" outlineLevel="0" r="15">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:28">
+    <row spans="1:28" outlineLevel="0" r="16">
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>

</xml_diff>

<commit_message>
fix giao diện hình ảnh web
</commit_message>
<xml_diff>
--- a/MauImport/MauImportQLTS - Copy.xlsx
+++ b/MauImport/MauImportQLTS - Copy.xlsx
@@ -7,30 +7,30 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="ViTri" sheetId="3" r:id="rId1"/>
-    <sheet name="NhanVienPT" sheetId="4" r:id="rId2"/>
-    <sheet name="Phong" sheetId="8" r:id="rId3"/>
-    <sheet name="LoaiThietBi" sheetId="5" r:id="rId4"/>
-    <sheet name="TinhTrang" sheetId="9" r:id="rId5"/>
-    <sheet name="ThietBiChung" sheetId="6" r:id="rId6"/>
-    <sheet name="ThietBiRieng" sheetId="10" r:id="rId7"/>
+    <sheet sheetId="3" r:id="rId1" name="ViTri"/>
+    <sheet sheetId="4" r:id="rId2" name="NhanVienPT"/>
+    <sheet sheetId="8" r:id="rId3" name="Phong"/>
+    <sheet sheetId="5" r:id="rId4" name="LoaiThietBi"/>
+    <sheet sheetId="9" r:id="rId5" name="TinhTrang"/>
+    <sheet sheetId="6" r:id="rId6" name="ThietBiChung"/>
+    <sheet sheetId="10" r:id="rId7" name="ThietBiRieng"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase">ViTri!$C$2:$C$18</definedName>
     <definedName name="Coso">#REF!:INDEX(#REF!,#REF!)</definedName>
     <definedName name="Day">#REF!:INDEX(#REF!,#REF!)</definedName>
-    <definedName name="_xlnm.Extract">ViTri!$D$3</definedName>
     <definedName name="ListCoSo">#REF!</definedName>
     <definedName name="ListDay">#REF!</definedName>
     <definedName name="ListTang">#REF!</definedName>
-    <definedName name="MaNhanVien">NhanVienPT!$B$2:$B$2995</definedName>
-    <definedName name="NhanVien">NhanVienPT!$C$2:$C$2995</definedName>
     <definedName name="Tang">#REF!:INDEX(#REF!,#REF!)</definedName>
     <definedName name="UniqueCoSo">ViTri!$C$2:INDEX(ViTri!$C$2:$C$2001,COUNTA(ViTri!$C$2:$C$2001))</definedName>
     <definedName name="UniqueDay">ViTri!$E$2:INDEX(ViTri!$E$2:$E$2001,COUNTA(ViTri!$E$2:$E$2001))</definedName>
     <definedName name="UniqueTang">ViTri!$G$2:INDEX(ViTri!$G$2:$G$2001,COUNTA(ViTri!$G$2:$G$2001))</definedName>
+    <definedName name="_xlnm._FilterDatabase">ViTri!$C$2:$C$18</definedName>
+    <definedName name="_xlnm.Extract">ViTri!$D$3</definedName>
+    <definedName name="MaNhanVien">NhanVienPT!$B$2:$B$2995</definedName>
+    <definedName name="NhanVien">NhanVienPT!$C$2:$C$2995</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1013,7 +1013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1205,11 +1205,7 @@
       <c r="J5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="K5" s="24"/>
     </row>
     <row spans="1:28" outlineLevel="0" r="6">
       <c r="A6" s="21">
@@ -1239,11 +1235,7 @@
       <c r="J6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="K6" s="24"/>
     </row>
     <row spans="1:28" outlineLevel="0" r="7">
       <c r="A7" s="21">
@@ -1268,11 +1260,7 @@
       <c r="J7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K7" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="K7" s="24"/>
     </row>
     <row spans="1:28" outlineLevel="0" r="8">
       <c r="A8" s="21">
@@ -1302,11 +1290,7 @@
       <c r="J8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="K8" s="24"/>
     </row>
     <row spans="1:28" outlineLevel="0" r="9">
       <c r="A9" s="21">
@@ -1336,11 +1320,7 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="K9" s="24"/>
     </row>
     <row spans="1:28" outlineLevel="0" r="10">
       <c r="A10" s="21">
@@ -1370,11 +1350,7 @@
       <c r="J10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="24" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="K10" s="24"/>
     </row>
     <row spans="1:28" outlineLevel="0" r="11">
       <c r="A11" s="21">

</xml_diff>